<commit_message>
Updated 15C solution mixing tables
-inputted equations to improve clarity
</commit_message>
<xml_diff>
--- a/Solution_recipes/pCa/pCa 15°C pH7.0 Recipe & Mixing Table Printouts/pCa_mixing_tables_pH70_15C.xlsx
+++ b/Solution_recipes/pCa/pCa 15°C pH7.0 Recipe & Mixing Table Printouts/pCa_mixing_tables_pH70_15C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinminton/Documents/GitHub/Protocols/Solution_recipes/pCa/pCa 15°C pH7.0 Recipe &amp; Mixing Table Printouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC726393-13FD-6543-AB02-DFFD5C5E2D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC99D50E-2AAD-A64A-8398-4929BCDADA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="6780" windowWidth="29080" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1420" yWindow="2700" windowWidth="29080" windowHeight="18440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mixing Chart " sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t>Large Volume Mixing Chart (pH 7.0 and 15 degrees Celsius)</t>
   </si>
@@ -67,12 +67,6 @@
     <t>/3</t>
   </si>
   <si>
-    <t>/4</t>
-  </si>
-  <si>
-    <t>/5</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
   </si>
   <si>
     <t>vials 5ml</t>
-  </si>
-  <si>
-    <t>5ml vials</t>
   </si>
   <si>
     <t>pH 7.0</t>
@@ -135,6 +126,27 @@
   <si>
     <t>For 0.5ml of Each pCa</t>
   </si>
+  <si>
+    <t>Proportion 9.0</t>
+  </si>
+  <si>
+    <t>Proportion 4.5</t>
+  </si>
+  <si>
+    <t># of Vials</t>
+  </si>
+  <si>
+    <t>Amt of 9.0</t>
+  </si>
+  <si>
+    <t>Amt of 4.5</t>
+  </si>
+  <si>
+    <t>Amt 90+45</t>
+  </si>
+  <si>
+    <t>&lt;- *will differ depending on total amt of stock prepared</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -187,11 +199,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -206,6 +255,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -486,90 +544,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="9" width="6.6640625" customWidth="1"/>
-    <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="14" width="6.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-    </row>
-    <row r="2" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10">
-        <v>90</v>
+      <c r="F2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="10">
-        <v>45</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="9"/>
-    </row>
-    <row r="3" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="11">
         <v>6.4</v>
       </c>
@@ -580,35 +610,24 @@
         <v>0.43833100000000003</v>
       </c>
       <c r="D3" s="10">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
-        <v>25</v>
-      </c>
-      <c r="F3" s="11">
-        <v>1.5</v>
+        <v>30</v>
+      </c>
+      <c r="E3" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="12">
+        <f>H3*B3</f>
+        <v>25.275105</v>
       </c>
       <c r="G3" s="12">
-        <v>21.062587499999999</v>
-      </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12">
-        <v>7.0208624999999998</v>
-      </c>
-      <c r="J3" s="12">
-        <v>16.437412500000001</v>
-      </c>
-      <c r="K3" s="12">
-        <v>8.2187062500000003</v>
-      </c>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>H3*C3</f>
+        <v>19.724895</v>
+      </c>
+      <c r="H3" s="12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>6.2</v>
       </c>
@@ -619,35 +638,24 @@
         <v>0.553983</v>
       </c>
       <c r="D4" s="10">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
         <v>30</v>
       </c>
-      <c r="F4" s="11">
-        <v>1.5</v>
+      <c r="E4" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F4" s="12">
+        <f>H4*B4</f>
+        <v>20.070765000000002</v>
       </c>
       <c r="G4" s="12">
-        <v>20.070765000000002</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12">
-        <v>6.6902549999999996</v>
-      </c>
-      <c r="J4" s="12">
+        <f>H4*C4</f>
         <v>24.929234999999998</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12">
-        <v>8.3097449999999995</v>
-      </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12">
+      <c r="H4" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11">
         <v>6.1</v>
       </c>
@@ -658,35 +666,24 @@
         <v>0.61035399999999995</v>
       </c>
       <c r="D5" s="10">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
-        <v>25</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1.5</v>
+        <v>30</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F5" s="12">
+        <f>H5*B5</f>
+        <v>17.53407</v>
       </c>
       <c r="G5" s="12">
-        <v>14.611725</v>
+        <f>H5*C5</f>
+        <v>27.465929999999997</v>
       </c>
       <c r="H5" s="12">
-        <v>7.3058624999999999</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12">
-        <v>22.888275</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12">
-        <v>7.6294250000000003</v>
-      </c>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="10">
         <v>6</v>
       </c>
@@ -697,35 +694,24 @@
         <v>0.66386699999999998</v>
       </c>
       <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
         <v>30</v>
       </c>
-      <c r="F6" s="11">
-        <v>1.5</v>
+      <c r="E6" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="12">
+        <f>H6*B6</f>
+        <v>15.125985</v>
       </c>
       <c r="G6" s="12">
-        <v>15.125985</v>
+        <f>H6*C6</f>
+        <v>29.874015</v>
       </c>
       <c r="H6" s="12">
-        <v>7.5629925</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12">
-        <v>29.874015</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12">
-        <v>9.958005</v>
-      </c>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="11">
         <v>5.9</v>
       </c>
@@ -736,35 +722,24 @@
         <v>0.71343500000000004</v>
       </c>
       <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
         <v>30</v>
       </c>
-      <c r="F7" s="11">
-        <v>1.5</v>
+      <c r="E7" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="12">
+        <f>H7*B7</f>
+        <v>12.895425000000001</v>
       </c>
       <c r="G7" s="12">
-        <v>12.895424999999999</v>
+        <f>H7*C7</f>
+        <v>32.104575000000004</v>
       </c>
       <c r="H7" s="12">
-        <v>6.4477124999999997</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12">
-        <v>32.104574999999997</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12">
-        <v>8.0261437499999992</v>
-      </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11">
         <v>5.8</v>
       </c>
@@ -775,35 +750,24 @@
         <v>0.75833499999999998</v>
       </c>
       <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10">
         <v>30</v>
       </c>
-      <c r="F8" s="11">
-        <v>1.5</v>
+      <c r="E8" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F8" s="12">
+        <f>H8*B8</f>
+        <v>10.874924999999999</v>
       </c>
       <c r="G8" s="12">
-        <v>10.874924999999999</v>
+        <f>H8*C8</f>
+        <v>34.125075000000002</v>
       </c>
       <c r="H8" s="12">
-        <v>5.4374624999999996</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12">
-        <v>34.125075000000002</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12">
-        <v>8.5312687500000006</v>
-      </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11">
         <v>5.7</v>
       </c>
@@ -814,33 +778,24 @@
         <v>0.79820899999999995</v>
       </c>
       <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10">
         <v>30</v>
       </c>
-      <c r="F9" s="11">
-        <v>1.5</v>
+      <c r="E9" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F9" s="12">
+        <f>H9*B9</f>
+        <v>9.0805950000000006</v>
       </c>
       <c r="G9" s="12">
-        <v>9.0805950000000006</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12">
+        <f>H9*C9</f>
         <v>35.919404999999998</v>
       </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12">
-        <v>8.9798512499999994</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12">
+      <c r="H9" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="11">
         <v>5.6</v>
       </c>
@@ -851,33 +806,24 @@
         <v>0.83302900000000002</v>
       </c>
       <c r="D10" s="10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
         <v>30</v>
       </c>
-      <c r="F10" s="11">
-        <v>1.5</v>
+      <c r="E10" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="12">
+        <f>H10*B10</f>
+        <v>7.5136950000000002</v>
       </c>
       <c r="G10" s="12">
-        <v>7.5136950000000002</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12">
+        <f>H10*C10</f>
         <v>37.486305000000002</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12">
-        <v>9.3715762500000004</v>
-      </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12">
+      <c r="H10" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="11">
         <v>5.5</v>
       </c>
@@ -888,33 +834,24 @@
         <v>0.86302100000000004</v>
       </c>
       <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10">
-        <v>15</v>
-      </c>
-      <c r="F11" s="11">
-        <v>1.5</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F11" s="12">
+        <f>H11*B11</f>
+        <v>6.1640549999999994</v>
       </c>
       <c r="G11" s="12">
-        <v>3.0820275000000001</v>
-      </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12">
-        <v>19.417972500000001</v>
-      </c>
-      <c r="K11" s="12">
-        <v>9.7089862500000006</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+        <f>H11*C11</f>
+        <v>38.835945000000002</v>
+      </c>
+      <c r="H11" s="12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="11">
         <v>5.4</v>
       </c>
@@ -925,33 +862,24 @@
         <v>0.88858700000000002</v>
       </c>
       <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="10">
         <v>30</v>
       </c>
-      <c r="F12" s="11">
-        <v>1.5</v>
+      <c r="E12" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="12">
+        <f>H12*B12</f>
+        <v>5.013585</v>
       </c>
       <c r="G12" s="12">
-        <v>5.013585</v>
-      </c>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12">
+        <f>H12*C12</f>
         <v>39.986415000000001</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12">
-        <v>9.9966037500000002</v>
-      </c>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12">
+      <c r="H12" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="11">
         <v>5.2</v>
       </c>
@@ -962,33 +890,24 @@
         <v>0.928485</v>
       </c>
       <c r="D13" s="10">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10">
         <v>30</v>
       </c>
-      <c r="F13" s="11">
-        <v>1.5</v>
+      <c r="E13" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F13" s="12">
+        <f>H13*B13</f>
+        <v>3.2181749999999996</v>
       </c>
       <c r="G13" s="12">
-        <v>3.218175</v>
-      </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12">
+        <f>H13*C13</f>
         <v>41.781824999999998</v>
       </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12">
-        <v>8.3563650000000003</v>
-      </c>
-      <c r="O13" s="12">
+      <c r="H13" s="12">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="10">
         <v>5</v>
       </c>
@@ -999,101 +918,74 @@
         <v>0.95696499999999995</v>
       </c>
       <c r="D14" s="10">
-        <v>1.0000004</v>
-      </c>
-      <c r="E14" s="10">
         <v>30</v>
       </c>
-      <c r="F14" s="11">
-        <v>1.5</v>
+      <c r="E14" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="12">
+        <f>H14*B14</f>
+        <v>1.9365937746371999</v>
       </c>
       <c r="G14" s="12">
-        <v>1.936593</v>
-      </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12">
-        <v>43.063425000000002</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12">
-        <v>8.6126850000000008</v>
-      </c>
-      <c r="O14" s="12">
+        <f>H14*C14</f>
+        <v>43.063442225369997</v>
+      </c>
+      <c r="H14" s="12">
         <v>45.000017999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F15" s="9" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="13">
+        <f>SUM(F3:F14)</f>
+        <v>134.70297377463723</v>
+      </c>
+      <c r="G15" s="13">
+        <v>378.013935</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="13">
+        <f>250-F15</f>
+        <v>115.29702622536277</v>
+      </c>
+      <c r="G16" s="13">
+        <f>500-G15</f>
+        <v>121.986065</v>
+      </c>
+      <c r="I16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E17" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="13">
-        <v>124.48608299999999</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="13">
-        <v>378.013935</v>
-      </c>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F16" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="13">
-        <v>125.51391700000001</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="13">
-        <v>121.986065</v>
-      </c>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F17" s="9" t="s">
-        <v>12</v>
+      <c r="F17" s="10">
+        <f>F16/5</f>
+        <v>23.059405245072554</v>
       </c>
       <c r="G17" s="10">
-        <v>27.891981555555599</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="10">
-        <v>27.1080144444444</v>
-      </c>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="19" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="20" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G20" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" spans="6:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G23" s="11">
-        <v>124.48608299999999</v>
-      </c>
-      <c r="J23" s="12">
-        <v>378.013935</v>
-      </c>
-    </row>
+        <f>G16/5</f>
+        <v>24.397213000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="20" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="21" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="22" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="23" spans="5:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1117,12 +1009,12 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1489,7 +1381,7 @@
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E19" s="5">
         <v>5.6528453399999998</v>
@@ -1524,12 +1416,12 @@
   <sheetData>
     <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2188,7 +2080,7 @@
     <row r="1" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="I1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2220,10 +2112,10 @@
         <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="P2" t="s">
         <v>5</v>
@@ -2874,7 +2766,7 @@
         <v>1.5</v>
       </c>
       <c r="P14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q14" s="4">
         <v>116.10636</v>
@@ -2906,7 +2798,7 @@
         <v>1.5</v>
       </c>
       <c r="P15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="4">
         <v>133.89364</v>
@@ -2938,7 +2830,7 @@
         <v>1.5</v>
       </c>
       <c r="P16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="Q16" s="4">
         <v>44.631213333333299</v>
@@ -3226,7 +3118,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4024,7 +3916,7 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D38" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E38" s="2">
         <v>5.2223670000000002</v>
@@ -4038,7 +3930,7 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2">
         <v>1.09713592436975</v>
@@ -4072,7 +3964,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4849,7 +4741,7 @@
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E39" s="2">
         <v>2.3495370000000002</v>
@@ -4863,7 +4755,7 @@
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E40" s="2">
         <v>0.49360021008402999</v>
@@ -4896,7 +4788,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5695,7 +5587,7 @@
     </row>
     <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D39" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E39" s="2">
         <v>2.3913634500000001</v>
@@ -5709,7 +5601,7 @@
     </row>
     <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E40" s="2">
         <v>0.50238727941175998</v>
@@ -5743,7 +5635,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6621,7 +6513,7 @@
     </row>
     <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D43" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E43" s="2">
         <v>3.6457514999999998</v>
@@ -6635,7 +6527,7 @@
     </row>
     <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E44" s="2">
         <v>0.76591418067227002</v>
@@ -6668,7 +6560,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7493,7 +7385,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -8324,7 +8216,7 @@
     </row>
     <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E37" s="8">
         <v>2.795223</v>
@@ -8335,7 +8227,7 @@
     </row>
     <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D38" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E38" s="2">
         <v>0.62116066666667002</v>
@@ -8369,7 +8261,7 @@
   <sheetData>
     <row r="1" spans="3:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="3:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8838,10 +8730,10 @@
     <row r="24" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="25" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H25" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="3:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9157,12 +9049,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LabArchives xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
-  <BaseUri>https://mynotebook.labarchives.com</BaseUri>
-  <eid>MzgzLjV8NjczMzIxLzI5NS9FbnRyeVBhcnQvMTcyNTY3NjA3MXw5NzMuNQ==</eid>
-  <version>1</version>
-  <updated-at>2022-02-15T10:48:35-05:00</updated-at>
-</LabArchives>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9389,12 +9281,12 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LabArchives xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema">
+  <BaseUri>https://mynotebook.labarchives.com</BaseUri>
+  <eid>MzgzLjV8NjczMzIxLzI5NS9FbnRyeVBhcnQvMTcyNTY3NjA3MXw5NzMuNQ==</eid>
+  <version>1</version>
+  <updated-at>2022-02-15T10:48:35-05:00</updated-at>
+</LabArchives>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9407,9 +9299,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B88236-9E0C-45FB-91E8-9D984BC38B29}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD22D77-2F70-4156-9D23-E02D1827EDD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9434,9 +9326,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACD22D77-2F70-4156-9D23-E02D1827EDD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B88236-9E0C-45FB-91E8-9D984BC38B29}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>